<commit_message>
excessively complicated (but functional) invoice object thing now exists
</commit_message>
<xml_diff>
--- a/data/data_1.xlsx
+++ b/data/data_1.xlsx
@@ -1,34 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28227"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jadon\OneDrive\Desktop\Javescript invoice\invoice-maker\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD555E91-FED2-4D65-8010-E2EFB3336C7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -134,10 +115,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="7" formatCode="&quot;$&quot;#,##0.00_);\(&quot;$&quot;#,##0.00\)"/>
-  </numFmts>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -149,7 +128,7 @@
     <font>
       <b/>
       <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFffffff"/>
       <name val="Times New Roman"/>
       <family val="2"/>
     </font>
@@ -161,33 +140,33 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFfa7d00"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFffffff"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFfa7d00"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFffffff"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -201,17 +180,17 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFa5a5a5"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFf2f2f2"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF70AD47"/>
+        <fgColor rgb="FF70ad47"/>
       </patternFill>
     </fill>
   </fills>
@@ -225,31 +204,31 @@
     </border>
     <border>
       <left style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF3f3f3f"/>
       </left>
       <right style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF3f3f3f"/>
       </right>
       <top style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF3f3f3f"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF3f3f3f"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF3f3f3f"/>
       </left>
       <right style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF3f3f3f"/>
       </right>
       <top style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </bottom>
       <diagonal/>
     </border>
@@ -265,37 +244,37 @@
       <right/>
       <top/>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FFff8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF7f7f7f"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF7f7f7f"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF7f7f7f"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF7f7f7f"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </left>
       <right style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </right>
       <top style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </bottom>
       <diagonal/>
     </border>
@@ -304,68 +283,67 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="18">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="7" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="7" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="7" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="7" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="7" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="7" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="7" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="7" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="7" fontId="5" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="7" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="5" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="7" fontId="6" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="7" applyNumberFormat="1" borderId="6" applyBorder="1" fontId="6" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="7" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="7" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="7" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="7" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="7" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="7" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="7" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="7" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="7" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf xfId="0" numFmtId="7" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -376,10 +354,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -417,71 +395,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -509,7 +487,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -532,11 +510,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -545,13 +523,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -561,7 +539,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -570,7 +548,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -579,7 +557,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -587,10 +565,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -655,36 +633,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:P290"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3:N4"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.44140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" style="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" style="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.44140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.88671875" style="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.33203125" style="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.6640625" style="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.6640625" style="16" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.5546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11" style="15" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="13.5546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="14" width="23.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="15" width="25.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="15" width="18.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="15" width="13.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="15" width="12.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="14" width="29.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="16" width="10.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="15" width="17.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="16" width="10.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="15" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="16" width="11.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="15" width="10.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="15" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="15" width="11.005" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="21.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -730,7 +707,7 @@
       <c r="O1" s="4"/>
       <c r="P1" s="4"/>
     </row>
-    <row r="2" spans="1:16" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="28.5">
       <c r="A2" s="5" t="s">
         <v>14</v>
       </c>
@@ -766,20 +743,17 @@
       </c>
       <c r="L2" s="8">
         <f>0.05*M2</f>
-        <v>2322</v>
       </c>
       <c r="M2" s="8">
         <f>G2+I2+K2</f>
-        <v>46440</v>
       </c>
       <c r="N2" s="9">
         <f>L2+M2</f>
-        <v>48762</v>
       </c>
       <c r="O2" s="10"/>
       <c r="P2" s="10"/>
     </row>
-    <row r="3" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="5" t="s">
         <v>22</v>
       </c>
@@ -807,36 +781,33 @@
       <c r="K3" s="7"/>
       <c r="L3" s="8">
         <f>0.05*M3</f>
-        <v>25</v>
       </c>
       <c r="M3" s="8">
         <f>G3+I3+K3</f>
-        <v>500</v>
       </c>
       <c r="N3" s="9">
         <f>L3+M3</f>
-        <v>525</v>
       </c>
       <c r="O3" s="10"/>
       <c r="P3" s="10"/>
     </row>
-    <row r="4" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+      <c r="A4" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="6" t="s">
         <v>30</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="5" t="s">
         <v>31</v>
       </c>
       <c r="G4" s="7">
@@ -845,27 +816,22 @@
       <c r="H4" s="11"/>
       <c r="I4" s="7"/>
       <c r="J4" s="11"/>
-      <c r="K4" s="7">
-        <v>600</v>
-      </c>
+      <c r="K4" s="7"/>
       <c r="L4" s="8">
         <f>0.05*M4</f>
-        <v>40</v>
       </c>
       <c r="M4" s="8">
         <f>G4+I4+K4</f>
-        <v>800</v>
       </c>
       <c r="N4" s="9">
         <f>L4+M4</f>
-        <v>840</v>
       </c>
       <c r="O4" s="10"/>
       <c r="P4" s="10"/>
     </row>
-    <row r="5" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="12"/>
-      <c r="B5" s="11"/>
+      <c r="B5" s="6"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
@@ -881,7 +847,7 @@
       <c r="O5" s="10"/>
       <c r="P5" s="10"/>
     </row>
-    <row r="6" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="12"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
@@ -899,7 +865,7 @@
       <c r="O6" s="10"/>
       <c r="P6" s="10"/>
     </row>
-    <row r="7" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="12"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
@@ -917,7 +883,7 @@
       <c r="O7" s="10"/>
       <c r="P7" s="10"/>
     </row>
-    <row r="8" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="12"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
@@ -935,7 +901,7 @@
       <c r="O8" s="10"/>
       <c r="P8" s="10"/>
     </row>
-    <row r="9" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="12"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
@@ -953,7 +919,7 @@
       <c r="O9" s="10"/>
       <c r="P9" s="10"/>
     </row>
-    <row r="10" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="12"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -971,7 +937,7 @@
       <c r="O10" s="10"/>
       <c r="P10" s="10"/>
     </row>
-    <row r="11" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="12"/>
       <c r="B11" s="11"/>
       <c r="C11" s="11"/>
@@ -989,7 +955,7 @@
       <c r="O11" s="10"/>
       <c r="P11" s="10"/>
     </row>
-    <row r="12" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="12"/>
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
@@ -1007,7 +973,7 @@
       <c r="O12" s="10"/>
       <c r="P12" s="10"/>
     </row>
-    <row r="13" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="12"/>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
@@ -1025,7 +991,7 @@
       <c r="O13" s="10"/>
       <c r="P13" s="10"/>
     </row>
-    <row r="14" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="12"/>
       <c r="B14" s="11"/>
       <c r="C14" s="11"/>
@@ -1043,7 +1009,7 @@
       <c r="O14" s="10"/>
       <c r="P14" s="10"/>
     </row>
-    <row r="15" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="12"/>
       <c r="B15" s="11"/>
       <c r="C15" s="11"/>
@@ -1061,7 +1027,7 @@
       <c r="O15" s="10"/>
       <c r="P15" s="10"/>
     </row>
-    <row r="16" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="12"/>
       <c r="B16" s="11"/>
       <c r="C16" s="11"/>
@@ -1079,7 +1045,7 @@
       <c r="O16" s="10"/>
       <c r="P16" s="10"/>
     </row>
-    <row r="17" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="12"/>
       <c r="B17" s="11"/>
       <c r="C17" s="11"/>
@@ -1097,7 +1063,7 @@
       <c r="O17" s="10"/>
       <c r="P17" s="10"/>
     </row>
-    <row r="18" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="12"/>
       <c r="B18" s="11"/>
       <c r="C18" s="11"/>
@@ -1115,7 +1081,7 @@
       <c r="O18" s="10"/>
       <c r="P18" s="10"/>
     </row>
-    <row r="19" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="12"/>
       <c r="B19" s="11"/>
       <c r="C19" s="11"/>
@@ -1133,7 +1099,7 @@
       <c r="O19" s="10"/>
       <c r="P19" s="10"/>
     </row>
-    <row r="20" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="12"/>
       <c r="B20" s="11"/>
       <c r="C20" s="11"/>
@@ -1151,7 +1117,7 @@
       <c r="O20" s="10"/>
       <c r="P20" s="10"/>
     </row>
-    <row r="21" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="12"/>
       <c r="B21" s="11"/>
       <c r="C21" s="11"/>
@@ -1169,7 +1135,7 @@
       <c r="O21" s="10"/>
       <c r="P21" s="10"/>
     </row>
-    <row r="22" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="12"/>
       <c r="B22" s="11"/>
       <c r="C22" s="11"/>
@@ -1187,7 +1153,7 @@
       <c r="O22" s="10"/>
       <c r="P22" s="10"/>
     </row>
-    <row r="23" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="12"/>
       <c r="B23" s="11"/>
       <c r="C23" s="11"/>
@@ -1205,7 +1171,7 @@
       <c r="O23" s="10"/>
       <c r="P23" s="10"/>
     </row>
-    <row r="24" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="12"/>
       <c r="B24" s="11"/>
       <c r="C24" s="11"/>
@@ -1223,7 +1189,7 @@
       <c r="O24" s="10"/>
       <c r="P24" s="10"/>
     </row>
-    <row r="25" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="12"/>
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
@@ -1241,7 +1207,7 @@
       <c r="O25" s="10"/>
       <c r="P25" s="10"/>
     </row>
-    <row r="26" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
       <c r="A26" s="12"/>
       <c r="B26" s="11"/>
       <c r="C26" s="11"/>
@@ -1259,7 +1225,7 @@
       <c r="O26" s="10"/>
       <c r="P26" s="10"/>
     </row>
-    <row r="27" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
       <c r="A27" s="12"/>
       <c r="B27" s="11"/>
       <c r="C27" s="11"/>
@@ -1277,7 +1243,7 @@
       <c r="O27" s="10"/>
       <c r="P27" s="10"/>
     </row>
-    <row r="28" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
       <c r="A28" s="12"/>
       <c r="B28" s="11"/>
       <c r="C28" s="11"/>
@@ -1295,7 +1261,7 @@
       <c r="O28" s="10"/>
       <c r="P28" s="10"/>
     </row>
-    <row r="29" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
       <c r="A29" s="12"/>
       <c r="B29" s="11"/>
       <c r="C29" s="11"/>
@@ -1313,7 +1279,7 @@
       <c r="O29" s="10"/>
       <c r="P29" s="10"/>
     </row>
-    <row r="30" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
       <c r="A30" s="12"/>
       <c r="B30" s="11"/>
       <c r="C30" s="11"/>
@@ -1331,7 +1297,7 @@
       <c r="O30" s="10"/>
       <c r="P30" s="10"/>
     </row>
-    <row r="31" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
       <c r="A31" s="12"/>
       <c r="B31" s="11"/>
       <c r="C31" s="11"/>
@@ -1349,7 +1315,7 @@
       <c r="O31" s="10"/>
       <c r="P31" s="10"/>
     </row>
-    <row r="32" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
       <c r="A32" s="12"/>
       <c r="B32" s="11"/>
       <c r="C32" s="11"/>
@@ -1367,7 +1333,7 @@
       <c r="O32" s="10"/>
       <c r="P32" s="10"/>
     </row>
-    <row r="33" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
       <c r="A33" s="12"/>
       <c r="B33" s="11"/>
       <c r="C33" s="11"/>
@@ -1385,7 +1351,7 @@
       <c r="O33" s="10"/>
       <c r="P33" s="10"/>
     </row>
-    <row r="34" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
       <c r="A34" s="12"/>
       <c r="B34" s="11"/>
       <c r="C34" s="11"/>
@@ -1403,7 +1369,7 @@
       <c r="O34" s="10"/>
       <c r="P34" s="10"/>
     </row>
-    <row r="35" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
       <c r="A35" s="12"/>
       <c r="B35" s="11"/>
       <c r="C35" s="11"/>
@@ -1421,7 +1387,7 @@
       <c r="O35" s="10"/>
       <c r="P35" s="10"/>
     </row>
-    <row r="36" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
       <c r="A36" s="12"/>
       <c r="B36" s="11"/>
       <c r="C36" s="11"/>
@@ -1439,7 +1405,7 @@
       <c r="O36" s="10"/>
       <c r="P36" s="10"/>
     </row>
-    <row r="37" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
       <c r="A37" s="12"/>
       <c r="B37" s="11"/>
       <c r="C37" s="11"/>
@@ -1457,7 +1423,7 @@
       <c r="O37" s="10"/>
       <c r="P37" s="10"/>
     </row>
-    <row r="38" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
       <c r="A38" s="12"/>
       <c r="B38" s="11"/>
       <c r="C38" s="11"/>
@@ -1475,7 +1441,7 @@
       <c r="O38" s="10"/>
       <c r="P38" s="10"/>
     </row>
-    <row r="39" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
       <c r="A39" s="12"/>
       <c r="B39" s="11"/>
       <c r="C39" s="11"/>
@@ -1493,7 +1459,7 @@
       <c r="O39" s="10"/>
       <c r="P39" s="10"/>
     </row>
-    <row r="40" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
       <c r="A40" s="12"/>
       <c r="B40" s="11"/>
       <c r="C40" s="11"/>
@@ -1511,7 +1477,7 @@
       <c r="O40" s="10"/>
       <c r="P40" s="10"/>
     </row>
-    <row r="41" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
       <c r="A41" s="12"/>
       <c r="B41" s="11"/>
       <c r="C41" s="11"/>
@@ -1529,7 +1495,7 @@
       <c r="O41" s="10"/>
       <c r="P41" s="10"/>
     </row>
-    <row r="42" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
       <c r="A42" s="12"/>
       <c r="B42" s="11"/>
       <c r="C42" s="11"/>
@@ -1547,7 +1513,7 @@
       <c r="O42" s="10"/>
       <c r="P42" s="10"/>
     </row>
-    <row r="43" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
       <c r="A43" s="12"/>
       <c r="B43" s="11"/>
       <c r="C43" s="11"/>
@@ -1565,7 +1531,7 @@
       <c r="O43" s="10"/>
       <c r="P43" s="10"/>
     </row>
-    <row r="44" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
       <c r="A44" s="12"/>
       <c r="B44" s="11"/>
       <c r="C44" s="11"/>
@@ -1583,7 +1549,7 @@
       <c r="O44" s="10"/>
       <c r="P44" s="10"/>
     </row>
-    <row r="45" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
       <c r="A45" s="12"/>
       <c r="B45" s="11"/>
       <c r="C45" s="11"/>
@@ -1601,7 +1567,7 @@
       <c r="O45" s="10"/>
       <c r="P45" s="10"/>
     </row>
-    <row r="46" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
       <c r="A46" s="12"/>
       <c r="B46" s="11"/>
       <c r="C46" s="11"/>
@@ -1619,7 +1585,7 @@
       <c r="O46" s="10"/>
       <c r="P46" s="10"/>
     </row>
-    <row r="47" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
       <c r="A47" s="12"/>
       <c r="B47" s="11"/>
       <c r="C47" s="11"/>
@@ -1637,7 +1603,7 @@
       <c r="O47" s="10"/>
       <c r="P47" s="10"/>
     </row>
-    <row r="48" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
       <c r="A48" s="12"/>
       <c r="B48" s="11"/>
       <c r="C48" s="11"/>
@@ -1655,7 +1621,7 @@
       <c r="O48" s="10"/>
       <c r="P48" s="10"/>
     </row>
-    <row r="49" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
       <c r="A49" s="12"/>
       <c r="B49" s="11"/>
       <c r="C49" s="11"/>
@@ -1673,7 +1639,7 @@
       <c r="O49" s="10"/>
       <c r="P49" s="10"/>
     </row>
-    <row r="50" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
       <c r="A50" s="12"/>
       <c r="B50" s="11"/>
       <c r="C50" s="11"/>
@@ -1691,7 +1657,7 @@
       <c r="O50" s="10"/>
       <c r="P50" s="10"/>
     </row>
-    <row r="51" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
       <c r="A51" s="12"/>
       <c r="B51" s="11"/>
       <c r="C51" s="11"/>
@@ -1709,7 +1675,7 @@
       <c r="O51" s="10"/>
       <c r="P51" s="10"/>
     </row>
-    <row r="52" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
       <c r="A52" s="12"/>
       <c r="B52" s="11"/>
       <c r="C52" s="11"/>
@@ -1727,7 +1693,7 @@
       <c r="O52" s="10"/>
       <c r="P52" s="10"/>
     </row>
-    <row r="53" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75">
       <c r="A53" s="12"/>
       <c r="B53" s="11"/>
       <c r="C53" s="11"/>
@@ -1745,7 +1711,7 @@
       <c r="O53" s="10"/>
       <c r="P53" s="10"/>
     </row>
-    <row r="54" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75">
       <c r="A54" s="12"/>
       <c r="B54" s="11"/>
       <c r="C54" s="11"/>
@@ -1763,7 +1729,7 @@
       <c r="O54" s="10"/>
       <c r="P54" s="10"/>
     </row>
-    <row r="55" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
       <c r="A55" s="12"/>
       <c r="B55" s="11"/>
       <c r="C55" s="11"/>
@@ -1781,7 +1747,7 @@
       <c r="O55" s="10"/>
       <c r="P55" s="10"/>
     </row>
-    <row r="56" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75">
       <c r="A56" s="12"/>
       <c r="B56" s="11"/>
       <c r="C56" s="11"/>
@@ -1799,7 +1765,7 @@
       <c r="O56" s="10"/>
       <c r="P56" s="10"/>
     </row>
-    <row r="57" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75">
       <c r="A57" s="12"/>
       <c r="B57" s="11"/>
       <c r="C57" s="11"/>
@@ -1817,7 +1783,7 @@
       <c r="O57" s="10"/>
       <c r="P57" s="10"/>
     </row>
-    <row r="58" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75">
       <c r="A58" s="12"/>
       <c r="B58" s="11"/>
       <c r="C58" s="11"/>
@@ -1835,7 +1801,7 @@
       <c r="O58" s="10"/>
       <c r="P58" s="10"/>
     </row>
-    <row r="59" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75">
       <c r="A59" s="12"/>
       <c r="B59" s="11"/>
       <c r="C59" s="11"/>
@@ -1853,7 +1819,7 @@
       <c r="O59" s="10"/>
       <c r="P59" s="10"/>
     </row>
-    <row r="60" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75">
       <c r="A60" s="12"/>
       <c r="B60" s="11"/>
       <c r="C60" s="11"/>
@@ -1871,7 +1837,7 @@
       <c r="O60" s="10"/>
       <c r="P60" s="10"/>
     </row>
-    <row r="61" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75">
       <c r="A61" s="12"/>
       <c r="B61" s="11"/>
       <c r="C61" s="11"/>
@@ -1889,7 +1855,7 @@
       <c r="O61" s="10"/>
       <c r="P61" s="10"/>
     </row>
-    <row r="62" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75">
       <c r="A62" s="12"/>
       <c r="B62" s="11"/>
       <c r="C62" s="11"/>
@@ -1907,7 +1873,7 @@
       <c r="O62" s="13"/>
       <c r="P62" s="13"/>
     </row>
-    <row r="63" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75">
       <c r="A63" s="12"/>
       <c r="B63" s="11"/>
       <c r="C63" s="11"/>
@@ -1925,7 +1891,7 @@
       <c r="O63" s="13"/>
       <c r="P63" s="13"/>
     </row>
-    <row r="64" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="18.75">
       <c r="A64" s="12"/>
       <c r="B64" s="11"/>
       <c r="C64" s="11"/>
@@ -1943,7 +1909,7 @@
       <c r="O64" s="13"/>
       <c r="P64" s="13"/>
     </row>
-    <row r="65" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18.75">
       <c r="A65" s="12"/>
       <c r="B65" s="11"/>
       <c r="C65" s="11"/>
@@ -1961,7 +1927,7 @@
       <c r="O65" s="13"/>
       <c r="P65" s="13"/>
     </row>
-    <row r="66" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18.75">
       <c r="A66" s="12"/>
       <c r="B66" s="11"/>
       <c r="C66" s="11"/>
@@ -1979,7 +1945,7 @@
       <c r="O66" s="13"/>
       <c r="P66" s="13"/>
     </row>
-    <row r="67" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18.75">
       <c r="A67" s="12"/>
       <c r="B67" s="11"/>
       <c r="C67" s="11"/>
@@ -1997,7 +1963,7 @@
       <c r="O67" s="13"/>
       <c r="P67" s="13"/>
     </row>
-    <row r="68" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18.75">
       <c r="A68" s="12"/>
       <c r="B68" s="11"/>
       <c r="C68" s="11"/>
@@ -2015,7 +1981,7 @@
       <c r="O68" s="13"/>
       <c r="P68" s="13"/>
     </row>
-    <row r="69" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18.75">
       <c r="A69" s="12"/>
       <c r="B69" s="11"/>
       <c r="C69" s="11"/>
@@ -2033,7 +1999,7 @@
       <c r="O69" s="13"/>
       <c r="P69" s="13"/>
     </row>
-    <row r="70" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18.75">
       <c r="A70" s="12"/>
       <c r="B70" s="11"/>
       <c r="C70" s="11"/>
@@ -2051,7 +2017,7 @@
       <c r="O70" s="13"/>
       <c r="P70" s="13"/>
     </row>
-    <row r="71" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="18.75">
       <c r="A71" s="12"/>
       <c r="B71" s="11"/>
       <c r="C71" s="11"/>
@@ -2069,7 +2035,7 @@
       <c r="O71" s="13"/>
       <c r="P71" s="13"/>
     </row>
-    <row r="72" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="18.75">
       <c r="A72" s="12"/>
       <c r="B72" s="11"/>
       <c r="C72" s="11"/>
@@ -2087,7 +2053,7 @@
       <c r="O72" s="13"/>
       <c r="P72" s="13"/>
     </row>
-    <row r="73" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="18.75">
       <c r="A73" s="12"/>
       <c r="B73" s="11"/>
       <c r="C73" s="11"/>
@@ -2105,7 +2071,7 @@
       <c r="O73" s="13"/>
       <c r="P73" s="13"/>
     </row>
-    <row r="74" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="18.75">
       <c r="A74" s="12"/>
       <c r="B74" s="11"/>
       <c r="C74" s="11"/>
@@ -2123,7 +2089,7 @@
       <c r="O74" s="13"/>
       <c r="P74" s="13"/>
     </row>
-    <row r="75" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="18.75">
       <c r="A75" s="12"/>
       <c r="B75" s="11"/>
       <c r="C75" s="11"/>
@@ -2141,7 +2107,7 @@
       <c r="O75" s="13"/>
       <c r="P75" s="13"/>
     </row>
-    <row r="76" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="18.75">
       <c r="A76" s="12"/>
       <c r="B76" s="11"/>
       <c r="C76" s="11"/>
@@ -2159,7 +2125,7 @@
       <c r="O76" s="13"/>
       <c r="P76" s="13"/>
     </row>
-    <row r="77" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18.75">
       <c r="A77" s="12"/>
       <c r="B77" s="11"/>
       <c r="C77" s="11"/>
@@ -2177,7 +2143,7 @@
       <c r="O77" s="13"/>
       <c r="P77" s="13"/>
     </row>
-    <row r="78" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18.75">
       <c r="A78" s="12"/>
       <c r="B78" s="11"/>
       <c r="C78" s="11"/>
@@ -2195,7 +2161,7 @@
       <c r="O78" s="13"/>
       <c r="P78" s="13"/>
     </row>
-    <row r="79" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18.75">
       <c r="A79" s="12"/>
       <c r="B79" s="11"/>
       <c r="C79" s="11"/>
@@ -2213,7 +2179,7 @@
       <c r="O79" s="13"/>
       <c r="P79" s="13"/>
     </row>
-    <row r="80" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="18.75">
       <c r="A80" s="12"/>
       <c r="B80" s="11"/>
       <c r="C80" s="11"/>
@@ -2231,7 +2197,7 @@
       <c r="O80" s="13"/>
       <c r="P80" s="13"/>
     </row>
-    <row r="81" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="18.75">
       <c r="A81" s="12"/>
       <c r="B81" s="11"/>
       <c r="C81" s="11"/>
@@ -2249,7 +2215,7 @@
       <c r="O81" s="13"/>
       <c r="P81" s="13"/>
     </row>
-    <row r="82" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="18.75">
       <c r="A82" s="12"/>
       <c r="B82" s="11"/>
       <c r="C82" s="11"/>
@@ -2267,7 +2233,7 @@
       <c r="O82" s="13"/>
       <c r="P82" s="13"/>
     </row>
-    <row r="83" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="18.75">
       <c r="A83" s="12"/>
       <c r="B83" s="11"/>
       <c r="C83" s="11"/>
@@ -2285,7 +2251,7 @@
       <c r="O83" s="13"/>
       <c r="P83" s="13"/>
     </row>
-    <row r="84" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="18.75">
       <c r="A84" s="12"/>
       <c r="B84" s="11"/>
       <c r="C84" s="11"/>
@@ -2303,7 +2269,7 @@
       <c r="O84" s="13"/>
       <c r="P84" s="13"/>
     </row>
-    <row r="85" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="18.75">
       <c r="A85" s="12"/>
       <c r="B85" s="11"/>
       <c r="C85" s="11"/>
@@ -2321,7 +2287,7 @@
       <c r="O85" s="13"/>
       <c r="P85" s="13"/>
     </row>
-    <row r="86" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="18.75">
       <c r="A86" s="12"/>
       <c r="B86" s="11"/>
       <c r="C86" s="11"/>
@@ -2339,7 +2305,7 @@
       <c r="O86" s="13"/>
       <c r="P86" s="13"/>
     </row>
-    <row r="87" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="18.75">
       <c r="A87" s="12"/>
       <c r="B87" s="11"/>
       <c r="C87" s="11"/>
@@ -2357,7 +2323,7 @@
       <c r="O87" s="13"/>
       <c r="P87" s="13"/>
     </row>
-    <row r="88" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="18.75">
       <c r="A88" s="12"/>
       <c r="B88" s="11"/>
       <c r="C88" s="11"/>
@@ -2375,7 +2341,7 @@
       <c r="O88" s="13"/>
       <c r="P88" s="13"/>
     </row>
-    <row r="89" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="18.75">
       <c r="A89" s="12"/>
       <c r="B89" s="11"/>
       <c r="C89" s="11"/>
@@ -2393,7 +2359,7 @@
       <c r="O89" s="13"/>
       <c r="P89" s="13"/>
     </row>
-    <row r="90" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="18.75">
       <c r="A90" s="12"/>
       <c r="B90" s="11"/>
       <c r="C90" s="11"/>
@@ -2411,7 +2377,7 @@
       <c r="O90" s="13"/>
       <c r="P90" s="13"/>
     </row>
-    <row r="91" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="18.75">
       <c r="A91" s="12"/>
       <c r="B91" s="11"/>
       <c r="C91" s="11"/>
@@ -2429,7 +2395,7 @@
       <c r="O91" s="13"/>
       <c r="P91" s="13"/>
     </row>
-    <row r="92" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="18.75">
       <c r="A92" s="12"/>
       <c r="B92" s="11"/>
       <c r="C92" s="11"/>
@@ -2447,7 +2413,7 @@
       <c r="O92" s="13"/>
       <c r="P92" s="13"/>
     </row>
-    <row r="93" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="18.75">
       <c r="A93" s="12"/>
       <c r="B93" s="11"/>
       <c r="C93" s="11"/>
@@ -2465,7 +2431,7 @@
       <c r="O93" s="13"/>
       <c r="P93" s="13"/>
     </row>
-    <row r="94" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="18.75">
       <c r="A94" s="12"/>
       <c r="B94" s="11"/>
       <c r="C94" s="11"/>
@@ -2483,7 +2449,7 @@
       <c r="O94" s="13"/>
       <c r="P94" s="13"/>
     </row>
-    <row r="95" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="18.75">
       <c r="A95" s="12"/>
       <c r="B95" s="11"/>
       <c r="C95" s="11"/>
@@ -2501,7 +2467,7 @@
       <c r="O95" s="13"/>
       <c r="P95" s="13"/>
     </row>
-    <row r="96" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="18.75">
       <c r="A96" s="12"/>
       <c r="B96" s="11"/>
       <c r="C96" s="11"/>
@@ -2519,7 +2485,7 @@
       <c r="O96" s="13"/>
       <c r="P96" s="13"/>
     </row>
-    <row r="97" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="18.75">
       <c r="A97" s="12"/>
       <c r="B97" s="11"/>
       <c r="C97" s="11"/>
@@ -2537,7 +2503,7 @@
       <c r="O97" s="13"/>
       <c r="P97" s="13"/>
     </row>
-    <row r="98" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="18.75">
       <c r="A98" s="12"/>
       <c r="B98" s="11"/>
       <c r="C98" s="11"/>
@@ -2555,7 +2521,7 @@
       <c r="O98" s="13"/>
       <c r="P98" s="13"/>
     </row>
-    <row r="99" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="18.75">
       <c r="A99" s="12"/>
       <c r="B99" s="11"/>
       <c r="C99" s="11"/>
@@ -2573,7 +2539,7 @@
       <c r="O99" s="13"/>
       <c r="P99" s="13"/>
     </row>
-    <row r="100" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="18.75">
       <c r="A100" s="12"/>
       <c r="B100" s="11"/>
       <c r="C100" s="11"/>
@@ -2591,7 +2557,7 @@
       <c r="O100" s="13"/>
       <c r="P100" s="13"/>
     </row>
-    <row r="101" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="18.75">
       <c r="A101" s="12"/>
       <c r="B101" s="11"/>
       <c r="C101" s="11"/>
@@ -2609,7 +2575,7 @@
       <c r="O101" s="13"/>
       <c r="P101" s="13"/>
     </row>
-    <row r="102" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="18.75">
       <c r="A102" s="12"/>
       <c r="B102" s="11"/>
       <c r="C102" s="11"/>
@@ -2627,7 +2593,7 @@
       <c r="O102" s="13"/>
       <c r="P102" s="13"/>
     </row>
-    <row r="103" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="18.75">
       <c r="A103" s="12"/>
       <c r="B103" s="11"/>
       <c r="C103" s="11"/>
@@ -2645,7 +2611,7 @@
       <c r="O103" s="13"/>
       <c r="P103" s="13"/>
     </row>
-    <row r="104" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="18.75">
       <c r="A104" s="12"/>
       <c r="B104" s="11"/>
       <c r="C104" s="11"/>
@@ -2663,7 +2629,7 @@
       <c r="O104" s="13"/>
       <c r="P104" s="13"/>
     </row>
-    <row r="105" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="18.75">
       <c r="A105" s="12"/>
       <c r="B105" s="11"/>
       <c r="C105" s="11"/>
@@ -2681,7 +2647,7 @@
       <c r="O105" s="13"/>
       <c r="P105" s="13"/>
     </row>
-    <row r="106" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="18.75">
       <c r="A106" s="12"/>
       <c r="B106" s="11"/>
       <c r="C106" s="11"/>
@@ -2699,7 +2665,7 @@
       <c r="O106" s="13"/>
       <c r="P106" s="13"/>
     </row>
-    <row r="107" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="18.75">
       <c r="A107" s="12"/>
       <c r="B107" s="11"/>
       <c r="C107" s="11"/>
@@ -2717,7 +2683,7 @@
       <c r="O107" s="13"/>
       <c r="P107" s="13"/>
     </row>
-    <row r="108" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="18.75">
       <c r="A108" s="12"/>
       <c r="B108" s="11"/>
       <c r="C108" s="11"/>
@@ -2735,7 +2701,7 @@
       <c r="O108" s="13"/>
       <c r="P108" s="13"/>
     </row>
-    <row r="109" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="18.75">
       <c r="A109" s="12"/>
       <c r="B109" s="11"/>
       <c r="C109" s="11"/>
@@ -2753,7 +2719,7 @@
       <c r="O109" s="13"/>
       <c r="P109" s="13"/>
     </row>
-    <row r="110" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="18.75">
       <c r="A110" s="12"/>
       <c r="B110" s="11"/>
       <c r="C110" s="11"/>
@@ -2771,7 +2737,7 @@
       <c r="O110" s="13"/>
       <c r="P110" s="13"/>
     </row>
-    <row r="111" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="18.75">
       <c r="A111" s="12"/>
       <c r="B111" s="11"/>
       <c r="C111" s="11"/>
@@ -2789,7 +2755,7 @@
       <c r="O111" s="13"/>
       <c r="P111" s="13"/>
     </row>
-    <row r="112" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="18.75">
       <c r="A112" s="12"/>
       <c r="B112" s="11"/>
       <c r="C112" s="11"/>
@@ -2807,7 +2773,7 @@
       <c r="O112" s="13"/>
       <c r="P112" s="13"/>
     </row>
-    <row r="113" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="113" customHeight="1" ht="18.75">
       <c r="A113" s="12"/>
       <c r="B113" s="11"/>
       <c r="C113" s="11"/>
@@ -2825,7 +2791,7 @@
       <c r="O113" s="13"/>
       <c r="P113" s="13"/>
     </row>
-    <row r="114" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="18.75">
       <c r="A114" s="12"/>
       <c r="B114" s="11"/>
       <c r="C114" s="11"/>
@@ -2843,7 +2809,7 @@
       <c r="O114" s="13"/>
       <c r="P114" s="13"/>
     </row>
-    <row r="115" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="115" customHeight="1" ht="18.75">
       <c r="A115" s="12"/>
       <c r="B115" s="11"/>
       <c r="C115" s="11"/>
@@ -2861,7 +2827,7 @@
       <c r="O115" s="13"/>
       <c r="P115" s="13"/>
     </row>
-    <row r="116" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="116" customHeight="1" ht="18.75">
       <c r="A116" s="12"/>
       <c r="B116" s="11"/>
       <c r="C116" s="11"/>
@@ -2879,7 +2845,7 @@
       <c r="O116" s="13"/>
       <c r="P116" s="13"/>
     </row>
-    <row r="117" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="117" customHeight="1" ht="18.75">
       <c r="A117" s="12"/>
       <c r="B117" s="11"/>
       <c r="C117" s="11"/>
@@ -2897,7 +2863,7 @@
       <c r="O117" s="13"/>
       <c r="P117" s="13"/>
     </row>
-    <row r="118" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="118" customHeight="1" ht="18.75">
       <c r="A118" s="12"/>
       <c r="B118" s="11"/>
       <c r="C118" s="11"/>
@@ -2915,7 +2881,7 @@
       <c r="O118" s="13"/>
       <c r="P118" s="13"/>
     </row>
-    <row r="119" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="119" customHeight="1" ht="18.75">
       <c r="A119" s="12"/>
       <c r="B119" s="11"/>
       <c r="C119" s="11"/>
@@ -2933,7 +2899,7 @@
       <c r="O119" s="13"/>
       <c r="P119" s="13"/>
     </row>
-    <row r="120" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="120" customHeight="1" ht="18.75">
       <c r="A120" s="12"/>
       <c r="B120" s="11"/>
       <c r="C120" s="11"/>
@@ -2951,7 +2917,7 @@
       <c r="O120" s="13"/>
       <c r="P120" s="13"/>
     </row>
-    <row r="121" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="121" customHeight="1" ht="18.75">
       <c r="A121" s="12"/>
       <c r="B121" s="11"/>
       <c r="C121" s="11"/>
@@ -2969,7 +2935,7 @@
       <c r="O121" s="13"/>
       <c r="P121" s="13"/>
     </row>
-    <row r="122" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="122" customHeight="1" ht="18.75">
       <c r="A122" s="12"/>
       <c r="B122" s="11"/>
       <c r="C122" s="11"/>
@@ -2987,7 +2953,7 @@
       <c r="O122" s="13"/>
       <c r="P122" s="13"/>
     </row>
-    <row r="123" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="123" customHeight="1" ht="18.75">
       <c r="A123" s="12"/>
       <c r="B123" s="11"/>
       <c r="C123" s="11"/>
@@ -3005,7 +2971,7 @@
       <c r="O123" s="13"/>
       <c r="P123" s="13"/>
     </row>
-    <row r="124" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="124" customHeight="1" ht="18.75">
       <c r="A124" s="12"/>
       <c r="B124" s="11"/>
       <c r="C124" s="11"/>
@@ -3023,7 +2989,7 @@
       <c r="O124" s="13"/>
       <c r="P124" s="13"/>
     </row>
-    <row r="125" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="125" customHeight="1" ht="18.75">
       <c r="A125" s="12"/>
       <c r="B125" s="11"/>
       <c r="C125" s="11"/>
@@ -3041,7 +3007,7 @@
       <c r="O125" s="13"/>
       <c r="P125" s="13"/>
     </row>
-    <row r="126" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="126" customHeight="1" ht="18.75">
       <c r="A126" s="12"/>
       <c r="B126" s="11"/>
       <c r="C126" s="11"/>
@@ -3059,7 +3025,7 @@
       <c r="O126" s="13"/>
       <c r="P126" s="13"/>
     </row>
-    <row r="127" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="127" customHeight="1" ht="18.75">
       <c r="A127" s="12"/>
       <c r="B127" s="11"/>
       <c r="C127" s="11"/>
@@ -3077,7 +3043,7 @@
       <c r="O127" s="13"/>
       <c r="P127" s="13"/>
     </row>
-    <row r="128" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="128" customHeight="1" ht="18.75">
       <c r="A128" s="12"/>
       <c r="B128" s="11"/>
       <c r="C128" s="11"/>
@@ -3095,7 +3061,7 @@
       <c r="O128" s="13"/>
       <c r="P128" s="13"/>
     </row>
-    <row r="129" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="129" customHeight="1" ht="18.75">
       <c r="A129" s="12"/>
       <c r="B129" s="11"/>
       <c r="C129" s="11"/>
@@ -3113,7 +3079,7 @@
       <c r="O129" s="13"/>
       <c r="P129" s="13"/>
     </row>
-    <row r="130" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="130" customHeight="1" ht="18.75">
       <c r="A130" s="12"/>
       <c r="B130" s="11"/>
       <c r="C130" s="11"/>
@@ -3131,7 +3097,7 @@
       <c r="O130" s="13"/>
       <c r="P130" s="13"/>
     </row>
-    <row r="131" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="131" customHeight="1" ht="18.75">
       <c r="A131" s="12"/>
       <c r="B131" s="11"/>
       <c r="C131" s="11"/>
@@ -3149,7 +3115,7 @@
       <c r="O131" s="13"/>
       <c r="P131" s="13"/>
     </row>
-    <row r="132" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="132" customHeight="1" ht="18.75">
       <c r="A132" s="12"/>
       <c r="B132" s="11"/>
       <c r="C132" s="11"/>
@@ -3167,7 +3133,7 @@
       <c r="O132" s="13"/>
       <c r="P132" s="13"/>
     </row>
-    <row r="133" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="133" customHeight="1" ht="18.75">
       <c r="A133" s="12"/>
       <c r="B133" s="11"/>
       <c r="C133" s="11"/>
@@ -3185,7 +3151,7 @@
       <c r="O133" s="13"/>
       <c r="P133" s="13"/>
     </row>
-    <row r="134" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="134" customHeight="1" ht="18.75">
       <c r="A134" s="12"/>
       <c r="B134" s="11"/>
       <c r="C134" s="11"/>
@@ -3203,7 +3169,7 @@
       <c r="O134" s="13"/>
       <c r="P134" s="13"/>
     </row>
-    <row r="135" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="135" customHeight="1" ht="18.75">
       <c r="A135" s="12"/>
       <c r="B135" s="11"/>
       <c r="C135" s="11"/>
@@ -3221,7 +3187,7 @@
       <c r="O135" s="13"/>
       <c r="P135" s="13"/>
     </row>
-    <row r="136" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="136" customHeight="1" ht="18.75">
       <c r="A136" s="12"/>
       <c r="B136" s="11"/>
       <c r="C136" s="11"/>
@@ -3239,7 +3205,7 @@
       <c r="O136" s="13"/>
       <c r="P136" s="13"/>
     </row>
-    <row r="137" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="137" customHeight="1" ht="18.75">
       <c r="A137" s="12"/>
       <c r="B137" s="11"/>
       <c r="C137" s="11"/>
@@ -3257,7 +3223,7 @@
       <c r="O137" s="13"/>
       <c r="P137" s="13"/>
     </row>
-    <row r="138" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="138" customHeight="1" ht="18.75">
       <c r="A138" s="12"/>
       <c r="B138" s="11"/>
       <c r="C138" s="11"/>
@@ -3275,7 +3241,7 @@
       <c r="O138" s="13"/>
       <c r="P138" s="13"/>
     </row>
-    <row r="139" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="139" customHeight="1" ht="18.75">
       <c r="A139" s="12"/>
       <c r="B139" s="11"/>
       <c r="C139" s="11"/>
@@ -3293,7 +3259,7 @@
       <c r="O139" s="13"/>
       <c r="P139" s="13"/>
     </row>
-    <row r="140" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="140" customHeight="1" ht="18.75">
       <c r="A140" s="12"/>
       <c r="B140" s="11"/>
       <c r="C140" s="11"/>
@@ -3311,7 +3277,7 @@
       <c r="O140" s="13"/>
       <c r="P140" s="13"/>
     </row>
-    <row r="141" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="141" customHeight="1" ht="18.75">
       <c r="A141" s="12"/>
       <c r="B141" s="11"/>
       <c r="C141" s="11"/>
@@ -3329,7 +3295,7 @@
       <c r="O141" s="13"/>
       <c r="P141" s="13"/>
     </row>
-    <row r="142" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="142" customHeight="1" ht="18.75">
       <c r="A142" s="12"/>
       <c r="B142" s="11"/>
       <c r="C142" s="11"/>
@@ -3347,7 +3313,7 @@
       <c r="O142" s="13"/>
       <c r="P142" s="13"/>
     </row>
-    <row r="143" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="143" customHeight="1" ht="18.75">
       <c r="A143" s="12"/>
       <c r="B143" s="11"/>
       <c r="C143" s="11"/>
@@ -3365,7 +3331,7 @@
       <c r="O143" s="13"/>
       <c r="P143" s="13"/>
     </row>
-    <row r="144" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="144" customHeight="1" ht="18.75">
       <c r="A144" s="12"/>
       <c r="B144" s="11"/>
       <c r="C144" s="11"/>
@@ -3383,7 +3349,7 @@
       <c r="O144" s="13"/>
       <c r="P144" s="13"/>
     </row>
-    <row r="145" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="145" customHeight="1" ht="18.75">
       <c r="A145" s="12"/>
       <c r="B145" s="11"/>
       <c r="C145" s="11"/>
@@ -3401,7 +3367,7 @@
       <c r="O145" s="13"/>
       <c r="P145" s="13"/>
     </row>
-    <row r="146" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="146" customHeight="1" ht="18.75">
       <c r="A146" s="12"/>
       <c r="B146" s="11"/>
       <c r="C146" s="11"/>
@@ -3419,7 +3385,7 @@
       <c r="O146" s="13"/>
       <c r="P146" s="13"/>
     </row>
-    <row r="147" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="147" customHeight="1" ht="18.75">
       <c r="A147" s="12"/>
       <c r="B147" s="11"/>
       <c r="C147" s="11"/>
@@ -3437,7 +3403,7 @@
       <c r="O147" s="13"/>
       <c r="P147" s="13"/>
     </row>
-    <row r="148" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="148" customHeight="1" ht="18.75">
       <c r="A148" s="12"/>
       <c r="B148" s="11"/>
       <c r="C148" s="11"/>
@@ -3455,7 +3421,7 @@
       <c r="O148" s="13"/>
       <c r="P148" s="13"/>
     </row>
-    <row r="149" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="149" customHeight="1" ht="18.75">
       <c r="A149" s="12"/>
       <c r="B149" s="11"/>
       <c r="C149" s="11"/>
@@ -3473,7 +3439,7 @@
       <c r="O149" s="13"/>
       <c r="P149" s="13"/>
     </row>
-    <row r="150" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="150" customHeight="1" ht="18.75">
       <c r="A150" s="12"/>
       <c r="B150" s="11"/>
       <c r="C150" s="11"/>
@@ -3491,7 +3457,7 @@
       <c r="O150" s="13"/>
       <c r="P150" s="13"/>
     </row>
-    <row r="151" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="151" customHeight="1" ht="18.75">
       <c r="A151" s="12"/>
       <c r="B151" s="11"/>
       <c r="C151" s="11"/>
@@ -3509,7 +3475,7 @@
       <c r="O151" s="13"/>
       <c r="P151" s="13"/>
     </row>
-    <row r="152" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="152" customHeight="1" ht="18.75">
       <c r="A152" s="12"/>
       <c r="B152" s="11"/>
       <c r="C152" s="11"/>
@@ -3527,7 +3493,7 @@
       <c r="O152" s="13"/>
       <c r="P152" s="13"/>
     </row>
-    <row r="153" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="153" customHeight="1" ht="18.75">
       <c r="A153" s="12"/>
       <c r="B153" s="11"/>
       <c r="C153" s="11"/>
@@ -3545,7 +3511,7 @@
       <c r="O153" s="13"/>
       <c r="P153" s="13"/>
     </row>
-    <row r="154" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="154" customHeight="1" ht="18.75">
       <c r="A154" s="12"/>
       <c r="B154" s="11"/>
       <c r="C154" s="11"/>
@@ -3563,7 +3529,7 @@
       <c r="O154" s="13"/>
       <c r="P154" s="13"/>
     </row>
-    <row r="155" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="155" customHeight="1" ht="18.75">
       <c r="A155" s="12"/>
       <c r="B155" s="11"/>
       <c r="C155" s="11"/>
@@ -3581,7 +3547,7 @@
       <c r="O155" s="13"/>
       <c r="P155" s="13"/>
     </row>
-    <row r="156" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="156" customHeight="1" ht="18.75">
       <c r="A156" s="12"/>
       <c r="B156" s="11"/>
       <c r="C156" s="11"/>
@@ -3599,7 +3565,7 @@
       <c r="O156" s="13"/>
       <c r="P156" s="13"/>
     </row>
-    <row r="157" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="157" customHeight="1" ht="18.75">
       <c r="A157" s="12"/>
       <c r="B157" s="11"/>
       <c r="C157" s="11"/>
@@ -3617,7 +3583,7 @@
       <c r="O157" s="13"/>
       <c r="P157" s="13"/>
     </row>
-    <row r="158" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="158" customHeight="1" ht="18.75">
       <c r="A158" s="12"/>
       <c r="B158" s="11"/>
       <c r="C158" s="11"/>
@@ -3635,7 +3601,7 @@
       <c r="O158" s="13"/>
       <c r="P158" s="13"/>
     </row>
-    <row r="159" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="159" customHeight="1" ht="18.75">
       <c r="A159" s="12"/>
       <c r="B159" s="11"/>
       <c r="C159" s="11"/>
@@ -3653,7 +3619,7 @@
       <c r="O159" s="13"/>
       <c r="P159" s="13"/>
     </row>
-    <row r="160" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="160" customHeight="1" ht="18.75">
       <c r="A160" s="12"/>
       <c r="B160" s="11"/>
       <c r="C160" s="11"/>
@@ -3671,7 +3637,7 @@
       <c r="O160" s="13"/>
       <c r="P160" s="13"/>
     </row>
-    <row r="161" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="161" customHeight="1" ht="18.75">
       <c r="A161" s="12"/>
       <c r="B161" s="11"/>
       <c r="C161" s="11"/>
@@ -3689,7 +3655,7 @@
       <c r="O161" s="13"/>
       <c r="P161" s="13"/>
     </row>
-    <row r="162" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="162" customHeight="1" ht="18.75">
       <c r="A162" s="12"/>
       <c r="B162" s="11"/>
       <c r="C162" s="11"/>
@@ -3707,7 +3673,7 @@
       <c r="O162" s="13"/>
       <c r="P162" s="13"/>
     </row>
-    <row r="163" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="163" customHeight="1" ht="18.75">
       <c r="A163" s="12"/>
       <c r="B163" s="11"/>
       <c r="C163" s="11"/>
@@ -3725,7 +3691,7 @@
       <c r="O163" s="13"/>
       <c r="P163" s="13"/>
     </row>
-    <row r="164" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="164" customHeight="1" ht="18.75">
       <c r="A164" s="12"/>
       <c r="B164" s="11"/>
       <c r="C164" s="11"/>
@@ -3743,7 +3709,7 @@
       <c r="O164" s="13"/>
       <c r="P164" s="13"/>
     </row>
-    <row r="165" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="165" customHeight="1" ht="18.75">
       <c r="A165" s="12"/>
       <c r="B165" s="11"/>
       <c r="C165" s="11"/>
@@ -3761,7 +3727,7 @@
       <c r="O165" s="13"/>
       <c r="P165" s="13"/>
     </row>
-    <row r="166" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="166" customHeight="1" ht="18.75">
       <c r="A166" s="12"/>
       <c r="B166" s="11"/>
       <c r="C166" s="11"/>
@@ -3779,7 +3745,7 @@
       <c r="O166" s="13"/>
       <c r="P166" s="13"/>
     </row>
-    <row r="167" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="167" customHeight="1" ht="18.75">
       <c r="A167" s="12"/>
       <c r="B167" s="11"/>
       <c r="C167" s="11"/>
@@ -3797,7 +3763,7 @@
       <c r="O167" s="13"/>
       <c r="P167" s="13"/>
     </row>
-    <row r="168" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="168" customHeight="1" ht="18.75">
       <c r="A168" s="12"/>
       <c r="B168" s="11"/>
       <c r="C168" s="11"/>
@@ -3815,7 +3781,7 @@
       <c r="O168" s="13"/>
       <c r="P168" s="13"/>
     </row>
-    <row r="169" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="169" customHeight="1" ht="18.75">
       <c r="A169" s="12"/>
       <c r="B169" s="11"/>
       <c r="C169" s="11"/>
@@ -3833,7 +3799,7 @@
       <c r="O169" s="13"/>
       <c r="P169" s="13"/>
     </row>
-    <row r="170" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="170" customHeight="1" ht="18.75">
       <c r="A170" s="12"/>
       <c r="B170" s="11"/>
       <c r="C170" s="11"/>
@@ -3851,7 +3817,7 @@
       <c r="O170" s="13"/>
       <c r="P170" s="13"/>
     </row>
-    <row r="171" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="171" customHeight="1" ht="18.75">
       <c r="A171" s="12"/>
       <c r="B171" s="11"/>
       <c r="C171" s="11"/>
@@ -3869,7 +3835,7 @@
       <c r="O171" s="13"/>
       <c r="P171" s="13"/>
     </row>
-    <row r="172" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="172" customHeight="1" ht="18.75">
       <c r="A172" s="12"/>
       <c r="B172" s="11"/>
       <c r="C172" s="11"/>
@@ -3887,7 +3853,7 @@
       <c r="O172" s="13"/>
       <c r="P172" s="13"/>
     </row>
-    <row r="173" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="173" customHeight="1" ht="18.75">
       <c r="A173" s="12"/>
       <c r="B173" s="11"/>
       <c r="C173" s="11"/>
@@ -3905,7 +3871,7 @@
       <c r="O173" s="13"/>
       <c r="P173" s="13"/>
     </row>
-    <row r="174" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="174" customHeight="1" ht="18.75">
       <c r="A174" s="12"/>
       <c r="B174" s="11"/>
       <c r="C174" s="11"/>
@@ -3923,7 +3889,7 @@
       <c r="O174" s="13"/>
       <c r="P174" s="13"/>
     </row>
-    <row r="175" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="175" customHeight="1" ht="18.75">
       <c r="A175" s="12"/>
       <c r="B175" s="11"/>
       <c r="C175" s="11"/>
@@ -3941,7 +3907,7 @@
       <c r="O175" s="13"/>
       <c r="P175" s="13"/>
     </row>
-    <row r="176" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="176" customHeight="1" ht="18.75">
       <c r="A176" s="12"/>
       <c r="B176" s="11"/>
       <c r="C176" s="11"/>
@@ -3959,7 +3925,7 @@
       <c r="O176" s="13"/>
       <c r="P176" s="13"/>
     </row>
-    <row r="177" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="177" customHeight="1" ht="19.5">
       <c r="A177" s="12"/>
       <c r="B177" s="11"/>
       <c r="C177" s="11"/>
@@ -3977,7 +3943,7 @@
       <c r="O177" s="13"/>
       <c r="P177" s="13"/>
     </row>
-    <row r="178" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="178" customHeight="1" ht="19.5">
       <c r="A178" s="12"/>
       <c r="B178" s="11"/>
       <c r="C178" s="11"/>
@@ -3995,7 +3961,7 @@
       <c r="O178" s="13"/>
       <c r="P178" s="13"/>
     </row>
-    <row r="179" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="179" customHeight="1" ht="19.5">
       <c r="A179" s="12"/>
       <c r="B179" s="11"/>
       <c r="C179" s="11"/>
@@ -4013,7 +3979,7 @@
       <c r="O179" s="13"/>
       <c r="P179" s="13"/>
     </row>
-    <row r="180" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="180" customHeight="1" ht="19.5">
       <c r="A180" s="12"/>
       <c r="B180" s="11"/>
       <c r="C180" s="11"/>
@@ -4031,7 +3997,7 @@
       <c r="O180" s="13"/>
       <c r="P180" s="13"/>
     </row>
-    <row r="181" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="181" customHeight="1" ht="19.5">
       <c r="A181" s="12"/>
       <c r="B181" s="11"/>
       <c r="C181" s="11"/>
@@ -4049,7 +4015,7 @@
       <c r="O181" s="13"/>
       <c r="P181" s="13"/>
     </row>
-    <row r="182" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="182" customHeight="1" ht="19.5">
       <c r="A182" s="12"/>
       <c r="B182" s="11"/>
       <c r="C182" s="11"/>
@@ -4067,7 +4033,7 @@
       <c r="O182" s="13"/>
       <c r="P182" s="13"/>
     </row>
-    <row r="183" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="183" customHeight="1" ht="19.5">
       <c r="A183" s="12"/>
       <c r="B183" s="11"/>
       <c r="C183" s="11"/>
@@ -4085,7 +4051,7 @@
       <c r="O183" s="13"/>
       <c r="P183" s="13"/>
     </row>
-    <row r="184" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="184" customHeight="1" ht="19.5">
       <c r="A184" s="12"/>
       <c r="B184" s="11"/>
       <c r="C184" s="11"/>
@@ -4103,7 +4069,7 @@
       <c r="O184" s="13"/>
       <c r="P184" s="13"/>
     </row>
-    <row r="185" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="185" customHeight="1" ht="19.5">
       <c r="A185" s="12"/>
       <c r="B185" s="11"/>
       <c r="C185" s="11"/>
@@ -4121,7 +4087,7 @@
       <c r="O185" s="13"/>
       <c r="P185" s="13"/>
     </row>
-    <row r="186" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="186" customHeight="1" ht="19.5">
       <c r="A186" s="12"/>
       <c r="B186" s="11"/>
       <c r="C186" s="11"/>
@@ -4139,7 +4105,7 @@
       <c r="O186" s="13"/>
       <c r="P186" s="13"/>
     </row>
-    <row r="187" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="187" customHeight="1" ht="19.5">
       <c r="A187" s="12"/>
       <c r="B187" s="11"/>
       <c r="C187" s="11"/>
@@ -4157,7 +4123,7 @@
       <c r="O187" s="13"/>
       <c r="P187" s="13"/>
     </row>
-    <row r="188" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="188" customHeight="1" ht="19.5">
       <c r="A188" s="12"/>
       <c r="B188" s="11"/>
       <c r="C188" s="11"/>
@@ -4175,7 +4141,7 @@
       <c r="O188" s="13"/>
       <c r="P188" s="13"/>
     </row>
-    <row r="189" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="189" customHeight="1" ht="19.5">
       <c r="A189" s="12"/>
       <c r="B189" s="11"/>
       <c r="C189" s="11"/>
@@ -4193,7 +4159,7 @@
       <c r="O189" s="13"/>
       <c r="P189" s="13"/>
     </row>
-    <row r="190" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="190" customHeight="1" ht="19.5">
       <c r="A190" s="12"/>
       <c r="B190" s="11"/>
       <c r="C190" s="11"/>
@@ -4211,7 +4177,7 @@
       <c r="O190" s="13"/>
       <c r="P190" s="13"/>
     </row>
-    <row r="191" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="191" customHeight="1" ht="19.5">
       <c r="A191" s="12"/>
       <c r="B191" s="11"/>
       <c r="C191" s="11"/>
@@ -4229,7 +4195,7 @@
       <c r="O191" s="13"/>
       <c r="P191" s="13"/>
     </row>
-    <row r="192" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="192" customHeight="1" ht="19.5">
       <c r="A192" s="12"/>
       <c r="B192" s="11"/>
       <c r="C192" s="11"/>
@@ -4247,7 +4213,7 @@
       <c r="O192" s="13"/>
       <c r="P192" s="13"/>
     </row>
-    <row r="193" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="193" customHeight="1" ht="19.5">
       <c r="A193" s="12"/>
       <c r="B193" s="11"/>
       <c r="C193" s="11"/>
@@ -4265,7 +4231,7 @@
       <c r="O193" s="13"/>
       <c r="P193" s="13"/>
     </row>
-    <row r="194" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="194" customHeight="1" ht="19.5">
       <c r="A194" s="12"/>
       <c r="B194" s="11"/>
       <c r="C194" s="11"/>
@@ -4283,7 +4249,7 @@
       <c r="O194" s="13"/>
       <c r="P194" s="13"/>
     </row>
-    <row r="195" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="195" customHeight="1" ht="19.5">
       <c r="A195" s="12"/>
       <c r="B195" s="11"/>
       <c r="C195" s="11"/>
@@ -4301,7 +4267,7 @@
       <c r="O195" s="13"/>
       <c r="P195" s="13"/>
     </row>
-    <row r="196" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="196" customHeight="1" ht="19.5">
       <c r="A196" s="12"/>
       <c r="B196" s="11"/>
       <c r="C196" s="11"/>
@@ -4319,7 +4285,7 @@
       <c r="O196" s="13"/>
       <c r="P196" s="13"/>
     </row>
-    <row r="197" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="197" customHeight="1" ht="19.5">
       <c r="A197" s="12"/>
       <c r="B197" s="11"/>
       <c r="C197" s="11"/>
@@ -4337,7 +4303,7 @@
       <c r="O197" s="13"/>
       <c r="P197" s="13"/>
     </row>
-    <row r="198" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="198" customHeight="1" ht="19.5">
       <c r="A198" s="12"/>
       <c r="B198" s="11"/>
       <c r="C198" s="11"/>
@@ -4355,7 +4321,7 @@
       <c r="O198" s="13"/>
       <c r="P198" s="13"/>
     </row>
-    <row r="199" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="199" customHeight="1" ht="19.5">
       <c r="A199" s="12"/>
       <c r="B199" s="11"/>
       <c r="C199" s="11"/>
@@ -4373,7 +4339,7 @@
       <c r="O199" s="13"/>
       <c r="P199" s="13"/>
     </row>
-    <row r="200" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="200" customHeight="1" ht="19.5">
       <c r="A200" s="12"/>
       <c r="B200" s="11"/>
       <c r="C200" s="11"/>
@@ -4391,7 +4357,7 @@
       <c r="O200" s="13"/>
       <c r="P200" s="13"/>
     </row>
-    <row r="201" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="201" customHeight="1" ht="19.5">
       <c r="A201" s="12"/>
       <c r="B201" s="11"/>
       <c r="C201" s="11"/>
@@ -4409,7 +4375,7 @@
       <c r="O201" s="13"/>
       <c r="P201" s="13"/>
     </row>
-    <row r="202" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="202" customHeight="1" ht="18.75">
       <c r="A202" s="12"/>
       <c r="B202" s="11"/>
       <c r="C202" s="11"/>
@@ -4427,7 +4393,7 @@
       <c r="O202" s="13"/>
       <c r="P202" s="13"/>
     </row>
-    <row r="203" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="203" customHeight="1" ht="18.75">
       <c r="A203" s="12"/>
       <c r="B203" s="11"/>
       <c r="C203" s="11"/>
@@ -4445,7 +4411,7 @@
       <c r="O203" s="13"/>
       <c r="P203" s="13"/>
     </row>
-    <row r="204" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="204" customHeight="1" ht="18.75">
       <c r="A204" s="12"/>
       <c r="B204" s="11"/>
       <c r="C204" s="11"/>
@@ -4463,7 +4429,7 @@
       <c r="O204" s="13"/>
       <c r="P204" s="13"/>
     </row>
-    <row r="205" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="205" customHeight="1" ht="18.75">
       <c r="A205" s="12"/>
       <c r="B205" s="11"/>
       <c r="C205" s="11"/>
@@ -4481,7 +4447,7 @@
       <c r="O205" s="13"/>
       <c r="P205" s="13"/>
     </row>
-    <row r="206" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="206" customHeight="1" ht="18.75">
       <c r="A206" s="12"/>
       <c r="B206" s="11"/>
       <c r="C206" s="11"/>
@@ -4499,7 +4465,7 @@
       <c r="O206" s="13"/>
       <c r="P206" s="13"/>
     </row>
-    <row r="207" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="207" customHeight="1" ht="18.75">
       <c r="A207" s="12"/>
       <c r="B207" s="11"/>
       <c r="C207" s="11"/>
@@ -4517,7 +4483,7 @@
       <c r="O207" s="13"/>
       <c r="P207" s="13"/>
     </row>
-    <row r="208" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="208" customHeight="1" ht="18.75">
       <c r="A208" s="12"/>
       <c r="B208" s="11"/>
       <c r="C208" s="11"/>
@@ -4535,7 +4501,7 @@
       <c r="O208" s="13"/>
       <c r="P208" s="13"/>
     </row>
-    <row r="209" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="209" customHeight="1" ht="18.75">
       <c r="A209" s="12"/>
       <c r="B209" s="11"/>
       <c r="C209" s="11"/>
@@ -4553,7 +4519,7 @@
       <c r="O209" s="13"/>
       <c r="P209" s="13"/>
     </row>
-    <row r="210" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="210" customHeight="1" ht="18.75">
       <c r="A210" s="12"/>
       <c r="B210" s="11"/>
       <c r="C210" s="11"/>
@@ -4571,7 +4537,7 @@
       <c r="O210" s="13"/>
       <c r="P210" s="13"/>
     </row>
-    <row r="211" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="211" customHeight="1" ht="18.75">
       <c r="A211" s="12"/>
       <c r="B211" s="11"/>
       <c r="C211" s="11"/>
@@ -4589,7 +4555,7 @@
       <c r="O211" s="13"/>
       <c r="P211" s="13"/>
     </row>
-    <row r="212" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="212" customHeight="1" ht="18.75">
       <c r="A212" s="12"/>
       <c r="B212" s="11"/>
       <c r="C212" s="11"/>
@@ -4607,7 +4573,7 @@
       <c r="O212" s="13"/>
       <c r="P212" s="13"/>
     </row>
-    <row r="213" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="213" customHeight="1" ht="18.75">
       <c r="A213" s="12"/>
       <c r="B213" s="11"/>
       <c r="C213" s="11"/>
@@ -4625,7 +4591,7 @@
       <c r="O213" s="13"/>
       <c r="P213" s="13"/>
     </row>
-    <row r="214" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="214" customHeight="1" ht="18.75">
       <c r="A214" s="12"/>
       <c r="B214" s="11"/>
       <c r="C214" s="11"/>
@@ -4643,7 +4609,7 @@
       <c r="O214" s="13"/>
       <c r="P214" s="13"/>
     </row>
-    <row r="215" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="215" customHeight="1" ht="18.75">
       <c r="A215" s="12"/>
       <c r="B215" s="11"/>
       <c r="C215" s="11"/>
@@ -4661,7 +4627,7 @@
       <c r="O215" s="13"/>
       <c r="P215" s="13"/>
     </row>
-    <row r="216" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="216" customHeight="1" ht="18.75">
       <c r="A216" s="12"/>
       <c r="B216" s="11"/>
       <c r="C216" s="11"/>
@@ -4679,7 +4645,7 @@
       <c r="O216" s="13"/>
       <c r="P216" s="13"/>
     </row>
-    <row r="217" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="217" customHeight="1" ht="18.75">
       <c r="A217" s="12"/>
       <c r="B217" s="11"/>
       <c r="C217" s="11"/>
@@ -4697,7 +4663,7 @@
       <c r="O217" s="13"/>
       <c r="P217" s="13"/>
     </row>
-    <row r="218" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="218" customHeight="1" ht="18.75">
       <c r="A218" s="12"/>
       <c r="B218" s="11"/>
       <c r="C218" s="11"/>
@@ -4715,7 +4681,7 @@
       <c r="O218" s="13"/>
       <c r="P218" s="13"/>
     </row>
-    <row r="219" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="219" customHeight="1" ht="18.75">
       <c r="A219" s="12"/>
       <c r="B219" s="11"/>
       <c r="C219" s="11"/>
@@ -4733,7 +4699,7 @@
       <c r="O219" s="13"/>
       <c r="P219" s="13"/>
     </row>
-    <row r="220" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="220" customHeight="1" ht="18.75">
       <c r="A220" s="12"/>
       <c r="B220" s="11"/>
       <c r="C220" s="11"/>
@@ -4751,7 +4717,7 @@
       <c r="O220" s="13"/>
       <c r="P220" s="13"/>
     </row>
-    <row r="221" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="221" customHeight="1" ht="18.75">
       <c r="A221" s="12"/>
       <c r="B221" s="11"/>
       <c r="C221" s="11"/>
@@ -4769,7 +4735,7 @@
       <c r="O221" s="13"/>
       <c r="P221" s="13"/>
     </row>
-    <row r="222" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="222" customHeight="1" ht="18.75">
       <c r="A222" s="12"/>
       <c r="B222" s="11"/>
       <c r="C222" s="11"/>
@@ -4787,7 +4753,7 @@
       <c r="O222" s="13"/>
       <c r="P222" s="13"/>
     </row>
-    <row r="223" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="223" customHeight="1" ht="18.75">
       <c r="A223" s="12"/>
       <c r="B223" s="11"/>
       <c r="C223" s="11"/>
@@ -4805,7 +4771,7 @@
       <c r="O223" s="13"/>
       <c r="P223" s="13"/>
     </row>
-    <row r="224" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="224" customHeight="1" ht="18.75">
       <c r="A224" s="12"/>
       <c r="B224" s="11"/>
       <c r="C224" s="11"/>
@@ -4823,7 +4789,7 @@
       <c r="O224" s="13"/>
       <c r="P224" s="13"/>
     </row>
-    <row r="225" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="225" customHeight="1" ht="18.75">
       <c r="A225" s="12"/>
       <c r="B225" s="11"/>
       <c r="C225" s="11"/>
@@ -4841,7 +4807,7 @@
       <c r="O225" s="13"/>
       <c r="P225" s="13"/>
     </row>
-    <row r="226" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="226" customHeight="1" ht="18.75">
       <c r="A226" s="12"/>
       <c r="B226" s="11"/>
       <c r="C226" s="11"/>
@@ -4859,7 +4825,7 @@
       <c r="O226" s="13"/>
       <c r="P226" s="13"/>
     </row>
-    <row r="227" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="227" customHeight="1" ht="18.75">
       <c r="A227" s="12"/>
       <c r="B227" s="11"/>
       <c r="C227" s="11"/>
@@ -4877,7 +4843,7 @@
       <c r="O227" s="13"/>
       <c r="P227" s="13"/>
     </row>
-    <row r="228" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="228" customHeight="1" ht="18.75">
       <c r="A228" s="12"/>
       <c r="B228" s="11"/>
       <c r="C228" s="11"/>
@@ -4895,7 +4861,7 @@
       <c r="O228" s="13"/>
       <c r="P228" s="13"/>
     </row>
-    <row r="229" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="229" customHeight="1" ht="18.75">
       <c r="A229" s="12"/>
       <c r="B229" s="11"/>
       <c r="C229" s="11"/>
@@ -4913,7 +4879,7 @@
       <c r="O229" s="13"/>
       <c r="P229" s="13"/>
     </row>
-    <row r="230" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="230" customHeight="1" ht="18.75">
       <c r="A230" s="12"/>
       <c r="B230" s="11"/>
       <c r="C230" s="11"/>
@@ -4931,7 +4897,7 @@
       <c r="O230" s="13"/>
       <c r="P230" s="13"/>
     </row>
-    <row r="231" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="231" customHeight="1" ht="18.75">
       <c r="A231" s="12"/>
       <c r="B231" s="11"/>
       <c r="C231" s="11"/>
@@ -4949,7 +4915,7 @@
       <c r="O231" s="13"/>
       <c r="P231" s="13"/>
     </row>
-    <row r="232" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="232" customHeight="1" ht="18.75">
       <c r="A232" s="12"/>
       <c r="B232" s="11"/>
       <c r="C232" s="11"/>
@@ -4967,7 +4933,7 @@
       <c r="O232" s="13"/>
       <c r="P232" s="13"/>
     </row>
-    <row r="233" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="233" customHeight="1" ht="18.75">
       <c r="A233" s="12"/>
       <c r="B233" s="11"/>
       <c r="C233" s="11"/>
@@ -4985,7 +4951,7 @@
       <c r="O233" s="13"/>
       <c r="P233" s="13"/>
     </row>
-    <row r="234" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="234" customHeight="1" ht="18.75">
       <c r="A234" s="12"/>
       <c r="B234" s="11"/>
       <c r="C234" s="11"/>
@@ -5003,7 +4969,7 @@
       <c r="O234" s="13"/>
       <c r="P234" s="13"/>
     </row>
-    <row r="235" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="235" customHeight="1" ht="18.75">
       <c r="A235" s="12"/>
       <c r="B235" s="11"/>
       <c r="C235" s="11"/>
@@ -5021,7 +4987,7 @@
       <c r="O235" s="13"/>
       <c r="P235" s="13"/>
     </row>
-    <row r="236" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="236" customHeight="1" ht="18.75">
       <c r="A236" s="12"/>
       <c r="B236" s="11"/>
       <c r="C236" s="11"/>
@@ -5039,7 +5005,7 @@
       <c r="O236" s="13"/>
       <c r="P236" s="13"/>
     </row>
-    <row r="237" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="237" customHeight="1" ht="18.75">
       <c r="A237" s="12"/>
       <c r="B237" s="11"/>
       <c r="C237" s="11"/>
@@ -5057,7 +5023,7 @@
       <c r="O237" s="13"/>
       <c r="P237" s="13"/>
     </row>
-    <row r="238" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="238" customHeight="1" ht="18.75">
       <c r="A238" s="12"/>
       <c r="B238" s="11"/>
       <c r="C238" s="11"/>
@@ -5075,7 +5041,7 @@
       <c r="O238" s="13"/>
       <c r="P238" s="13"/>
     </row>
-    <row r="239" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="239" customHeight="1" ht="18.75">
       <c r="A239" s="12"/>
       <c r="B239" s="11"/>
       <c r="C239" s="11"/>
@@ -5093,7 +5059,7 @@
       <c r="O239" s="13"/>
       <c r="P239" s="13"/>
     </row>
-    <row r="240" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="240" customHeight="1" ht="18.75">
       <c r="A240" s="12"/>
       <c r="B240" s="11"/>
       <c r="C240" s="11"/>
@@ -5111,7 +5077,7 @@
       <c r="O240" s="13"/>
       <c r="P240" s="13"/>
     </row>
-    <row r="241" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="241" customHeight="1" ht="18.75">
       <c r="A241" s="12"/>
       <c r="B241" s="11"/>
       <c r="C241" s="11"/>
@@ -5129,7 +5095,7 @@
       <c r="O241" s="13"/>
       <c r="P241" s="13"/>
     </row>
-    <row r="242" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="242" customHeight="1" ht="18.75">
       <c r="A242" s="12"/>
       <c r="B242" s="11"/>
       <c r="C242" s="11"/>
@@ -5147,7 +5113,7 @@
       <c r="O242" s="13"/>
       <c r="P242" s="13"/>
     </row>
-    <row r="243" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="243" customHeight="1" ht="18.75">
       <c r="A243" s="12"/>
       <c r="B243" s="11"/>
       <c r="C243" s="11"/>
@@ -5165,7 +5131,7 @@
       <c r="O243" s="13"/>
       <c r="P243" s="13"/>
     </row>
-    <row r="244" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="244" customHeight="1" ht="18.75">
       <c r="A244" s="12"/>
       <c r="B244" s="11"/>
       <c r="C244" s="11"/>
@@ -5183,7 +5149,7 @@
       <c r="O244" s="13"/>
       <c r="P244" s="13"/>
     </row>
-    <row r="245" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="245" customHeight="1" ht="18.75">
       <c r="A245" s="12"/>
       <c r="B245" s="11"/>
       <c r="C245" s="11"/>
@@ -5201,7 +5167,7 @@
       <c r="O245" s="13"/>
       <c r="P245" s="13"/>
     </row>
-    <row r="246" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="246" customHeight="1" ht="18.75">
       <c r="A246" s="12"/>
       <c r="B246" s="11"/>
       <c r="C246" s="11"/>
@@ -5219,7 +5185,7 @@
       <c r="O246" s="13"/>
       <c r="P246" s="13"/>
     </row>
-    <row r="247" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="247" customHeight="1" ht="18.75">
       <c r="A247" s="12"/>
       <c r="B247" s="11"/>
       <c r="C247" s="11"/>
@@ -5237,7 +5203,7 @@
       <c r="O247" s="13"/>
       <c r="P247" s="13"/>
     </row>
-    <row r="248" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="248" customHeight="1" ht="18.75">
       <c r="A248" s="12"/>
       <c r="B248" s="11"/>
       <c r="C248" s="11"/>
@@ -5255,7 +5221,7 @@
       <c r="O248" s="13"/>
       <c r="P248" s="13"/>
     </row>
-    <row r="249" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="249" customHeight="1" ht="18.75">
       <c r="A249" s="12"/>
       <c r="B249" s="11"/>
       <c r="C249" s="11"/>
@@ -5273,7 +5239,7 @@
       <c r="O249" s="13"/>
       <c r="P249" s="13"/>
     </row>
-    <row r="250" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="250" customHeight="1" ht="18.75">
       <c r="A250" s="12"/>
       <c r="B250" s="11"/>
       <c r="C250" s="11"/>
@@ -5291,7 +5257,7 @@
       <c r="O250" s="13"/>
       <c r="P250" s="13"/>
     </row>
-    <row r="251" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="251" customHeight="1" ht="18.75">
       <c r="A251" s="12"/>
       <c r="B251" s="11"/>
       <c r="C251" s="11"/>
@@ -5309,7 +5275,7 @@
       <c r="O251" s="13"/>
       <c r="P251" s="13"/>
     </row>
-    <row r="252" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="252" customHeight="1" ht="18.75">
       <c r="A252" s="12"/>
       <c r="B252" s="11"/>
       <c r="C252" s="11"/>
@@ -5327,7 +5293,7 @@
       <c r="O252" s="13"/>
       <c r="P252" s="13"/>
     </row>
-    <row r="253" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="253" customHeight="1" ht="18.75">
       <c r="A253" s="12"/>
       <c r="B253" s="11"/>
       <c r="C253" s="11"/>
@@ -5345,7 +5311,7 @@
       <c r="O253" s="13"/>
       <c r="P253" s="13"/>
     </row>
-    <row r="254" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="254" customHeight="1" ht="18.75">
       <c r="A254" s="12"/>
       <c r="B254" s="11"/>
       <c r="C254" s="11"/>
@@ -5363,7 +5329,7 @@
       <c r="O254" s="13"/>
       <c r="P254" s="13"/>
     </row>
-    <row r="255" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="255" customHeight="1" ht="18.75">
       <c r="A255" s="12"/>
       <c r="B255" s="11"/>
       <c r="C255" s="11"/>
@@ -5381,7 +5347,7 @@
       <c r="O255" s="13"/>
       <c r="P255" s="13"/>
     </row>
-    <row r="256" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="256" customHeight="1" ht="18.75">
       <c r="A256" s="12"/>
       <c r="B256" s="11"/>
       <c r="C256" s="11"/>
@@ -5399,7 +5365,7 @@
       <c r="O256" s="13"/>
       <c r="P256" s="13"/>
     </row>
-    <row r="257" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="257" customHeight="1" ht="18.75">
       <c r="A257" s="12"/>
       <c r="B257" s="11"/>
       <c r="C257" s="11"/>
@@ -5417,7 +5383,7 @@
       <c r="O257" s="13"/>
       <c r="P257" s="13"/>
     </row>
-    <row r="258" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="258" customHeight="1" ht="18.75">
       <c r="A258" s="12"/>
       <c r="B258" s="11"/>
       <c r="C258" s="11"/>
@@ -5435,7 +5401,7 @@
       <c r="O258" s="13"/>
       <c r="P258" s="13"/>
     </row>
-    <row r="259" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="259" customHeight="1" ht="18.75">
       <c r="A259" s="12"/>
       <c r="B259" s="11"/>
       <c r="C259" s="11"/>
@@ -5453,7 +5419,7 @@
       <c r="O259" s="13"/>
       <c r="P259" s="13"/>
     </row>
-    <row r="260" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="260" customHeight="1" ht="18.75">
       <c r="A260" s="12"/>
       <c r="B260" s="11"/>
       <c r="C260" s="11"/>
@@ -5471,7 +5437,7 @@
       <c r="O260" s="13"/>
       <c r="P260" s="13"/>
     </row>
-    <row r="261" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="261" customHeight="1" ht="18.75">
       <c r="A261" s="12"/>
       <c r="B261" s="11"/>
       <c r="C261" s="11"/>
@@ -5489,7 +5455,7 @@
       <c r="O261" s="13"/>
       <c r="P261" s="13"/>
     </row>
-    <row r="262" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="262" customHeight="1" ht="18.75">
       <c r="A262" s="12"/>
       <c r="B262" s="11"/>
       <c r="C262" s="11"/>
@@ -5507,7 +5473,7 @@
       <c r="O262" s="13"/>
       <c r="P262" s="13"/>
     </row>
-    <row r="263" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="263" customHeight="1" ht="18.75">
       <c r="A263" s="12"/>
       <c r="B263" s="11"/>
       <c r="C263" s="11"/>
@@ -5525,7 +5491,7 @@
       <c r="O263" s="13"/>
       <c r="P263" s="13"/>
     </row>
-    <row r="264" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="264" customHeight="1" ht="18.75">
       <c r="A264" s="12"/>
       <c r="B264" s="11"/>
       <c r="C264" s="11"/>
@@ -5543,7 +5509,7 @@
       <c r="O264" s="13"/>
       <c r="P264" s="13"/>
     </row>
-    <row r="265" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="265" customHeight="1" ht="18.75">
       <c r="A265" s="12"/>
       <c r="B265" s="11"/>
       <c r="C265" s="11"/>
@@ -5561,7 +5527,7 @@
       <c r="O265" s="13"/>
       <c r="P265" s="13"/>
     </row>
-    <row r="266" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="266" customHeight="1" ht="18.75">
       <c r="A266" s="12"/>
       <c r="B266" s="11"/>
       <c r="C266" s="11"/>
@@ -5579,7 +5545,7 @@
       <c r="O266" s="13"/>
       <c r="P266" s="13"/>
     </row>
-    <row r="267" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="267" customHeight="1" ht="18.75">
       <c r="A267" s="12"/>
       <c r="B267" s="11"/>
       <c r="C267" s="11"/>
@@ -5597,7 +5563,7 @@
       <c r="O267" s="13"/>
       <c r="P267" s="13"/>
     </row>
-    <row r="268" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="268" customHeight="1" ht="18.75">
       <c r="A268" s="12"/>
       <c r="B268" s="11"/>
       <c r="C268" s="11"/>
@@ -5615,7 +5581,7 @@
       <c r="O268" s="13"/>
       <c r="P268" s="13"/>
     </row>
-    <row r="269" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="269" customHeight="1" ht="18.75">
       <c r="A269" s="12"/>
       <c r="B269" s="11"/>
       <c r="C269" s="11"/>
@@ -5633,7 +5599,7 @@
       <c r="O269" s="13"/>
       <c r="P269" s="13"/>
     </row>
-    <row r="270" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="270" customHeight="1" ht="18.75">
       <c r="A270" s="12"/>
       <c r="B270" s="11"/>
       <c r="C270" s="11"/>
@@ -5651,7 +5617,7 @@
       <c r="O270" s="13"/>
       <c r="P270" s="13"/>
     </row>
-    <row r="271" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="271" customHeight="1" ht="18.75">
       <c r="A271" s="12"/>
       <c r="B271" s="11"/>
       <c r="C271" s="11"/>
@@ -5669,7 +5635,7 @@
       <c r="O271" s="13"/>
       <c r="P271" s="13"/>
     </row>
-    <row r="272" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="272" customHeight="1" ht="18.75">
       <c r="A272" s="12"/>
       <c r="B272" s="11"/>
       <c r="C272" s="11"/>
@@ -5687,7 +5653,7 @@
       <c r="O272" s="13"/>
       <c r="P272" s="13"/>
     </row>
-    <row r="273" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="273" customHeight="1" ht="18.75">
       <c r="A273" s="12"/>
       <c r="B273" s="11"/>
       <c r="C273" s="11"/>
@@ -5705,7 +5671,7 @@
       <c r="O273" s="13"/>
       <c r="P273" s="13"/>
     </row>
-    <row r="274" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="274" customHeight="1" ht="18.75">
       <c r="A274" s="12"/>
       <c r="B274" s="11"/>
       <c r="C274" s="11"/>
@@ -5723,7 +5689,7 @@
       <c r="O274" s="13"/>
       <c r="P274" s="13"/>
     </row>
-    <row r="275" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="275" customHeight="1" ht="18.75">
       <c r="A275" s="12"/>
       <c r="B275" s="11"/>
       <c r="C275" s="11"/>
@@ -5741,7 +5707,7 @@
       <c r="O275" s="13"/>
       <c r="P275" s="13"/>
     </row>
-    <row r="276" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="276" customHeight="1" ht="18.75">
       <c r="A276" s="12"/>
       <c r="B276" s="11"/>
       <c r="C276" s="11"/>
@@ -5759,7 +5725,7 @@
       <c r="O276" s="13"/>
       <c r="P276" s="13"/>
     </row>
-    <row r="277" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="277" customHeight="1" ht="18.75">
       <c r="A277" s="12"/>
       <c r="B277" s="11"/>
       <c r="C277" s="11"/>
@@ -5777,7 +5743,7 @@
       <c r="O277" s="13"/>
       <c r="P277" s="13"/>
     </row>
-    <row r="278" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="278" customHeight="1" ht="18.75">
       <c r="A278" s="12"/>
       <c r="B278" s="11"/>
       <c r="C278" s="11"/>
@@ -5795,7 +5761,7 @@
       <c r="O278" s="13"/>
       <c r="P278" s="13"/>
     </row>
-    <row r="279" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="279" customHeight="1" ht="18.75">
       <c r="A279" s="12"/>
       <c r="B279" s="11"/>
       <c r="C279" s="11"/>
@@ -5813,7 +5779,7 @@
       <c r="O279" s="13"/>
       <c r="P279" s="13"/>
     </row>
-    <row r="280" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="280" customHeight="1" ht="18.75">
       <c r="A280" s="12"/>
       <c r="B280" s="11"/>
       <c r="C280" s="11"/>
@@ -5831,7 +5797,7 @@
       <c r="O280" s="13"/>
       <c r="P280" s="13"/>
     </row>
-    <row r="281" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="281" customHeight="1" ht="18.75">
       <c r="A281" s="12"/>
       <c r="B281" s="11"/>
       <c r="C281" s="11"/>
@@ -5849,7 +5815,7 @@
       <c r="O281" s="13"/>
       <c r="P281" s="13"/>
     </row>
-    <row r="282" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="282" customHeight="1" ht="18.75">
       <c r="A282" s="12"/>
       <c r="B282" s="11"/>
       <c r="C282" s="11"/>
@@ -5867,7 +5833,7 @@
       <c r="O282" s="13"/>
       <c r="P282" s="13"/>
     </row>
-    <row r="283" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="283" customHeight="1" ht="18.75">
       <c r="A283" s="12"/>
       <c r="B283" s="11"/>
       <c r="C283" s="11"/>
@@ -5885,7 +5851,7 @@
       <c r="O283" s="13"/>
       <c r="P283" s="13"/>
     </row>
-    <row r="284" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="284" customHeight="1" ht="18.75">
       <c r="A284" s="12"/>
       <c r="B284" s="11"/>
       <c r="C284" s="11"/>
@@ -5903,7 +5869,7 @@
       <c r="O284" s="13"/>
       <c r="P284" s="13"/>
     </row>
-    <row r="285" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="285" customHeight="1" ht="18.75">
       <c r="A285" s="12"/>
       <c r="B285" s="11"/>
       <c r="C285" s="11"/>
@@ -5921,7 +5887,7 @@
       <c r="O285" s="13"/>
       <c r="P285" s="13"/>
     </row>
-    <row r="286" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="286" customHeight="1" ht="18.75">
       <c r="A286" s="12"/>
       <c r="B286" s="11"/>
       <c r="C286" s="11"/>
@@ -5939,7 +5905,7 @@
       <c r="O286" s="13"/>
       <c r="P286" s="13"/>
     </row>
-    <row r="287" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="287" customHeight="1" ht="18.75">
       <c r="A287" s="12"/>
       <c r="B287" s="11"/>
       <c r="C287" s="11"/>
@@ -5957,7 +5923,7 @@
       <c r="O287" s="13"/>
       <c r="P287" s="13"/>
     </row>
-    <row r="288" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="288" customHeight="1" ht="18.75">
       <c r="A288" s="12"/>
       <c r="B288" s="11"/>
       <c r="C288" s="11"/>
@@ -5975,7 +5941,7 @@
       <c r="O288" s="13"/>
       <c r="P288" s="13"/>
     </row>
-    <row r="289" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="289" customHeight="1" ht="18.75">
       <c r="A289" s="12"/>
       <c r="B289" s="11"/>
       <c r="C289" s="11"/>
@@ -5993,7 +5959,7 @@
       <c r="O289" s="13"/>
       <c r="P289" s="13"/>
     </row>
-    <row r="290" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="290" customHeight="1" ht="18.75">
       <c r="A290" s="12"/>
       <c r="B290" s="11"/>
       <c r="C290" s="11"/>

</xml_diff>